<commit_message>
Atualizacoes 16 de janeiro de 2024.
</commit_message>
<xml_diff>
--- a/StructureDefinition-EthnicityExtension.xlsx
+++ b/StructureDefinition-EthnicityExtension.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.1</t>
+    <t>0.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -42,7 +42,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Extension of Patient Ethnicity</t>
+    <t>Ethnicity</t>
   </si>
   <si>
     <t>Status</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-11-21T19:08:35-03:00</t>
+    <t>2024-01-16T20:08:55-03:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -75,7 +75,7 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Extension to capture the patient's ethnicity which represents their cultural background or heritage. Although optional, ICHOM strongly encourages collecting this inclusive information.</t>
+    <t>Extension to capture the patient's ethnicity which represents their cultural background or heritage.</t>
   </si>
   <si>
     <t>Purpose</t>

</xml_diff>